<commit_message>
Placa CRMaze_board_futura con forma y componente colocados
</commit_message>
<xml_diff>
--- a/Componentes.xlsx
+++ b/Componentes.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="6760" windowWidth="14400" windowHeight="9660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" calcMode="manual" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="4" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="63">
   <si>
     <t>Componente</t>
   </si>
@@ -140,12 +140,6 @@
     <t>MODE INDICATOR</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>Boton SMD</t>
   </si>
   <si>
@@ -186,6 +180,42 @@
   </si>
   <si>
     <t>Selección Componentes:</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/_/?Keyword=TPS73633+SOT-23&amp;FS=True</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/Semiconductors/Power-Management-ICs/Voltage-Regulators-Voltage-Controllers/LDO-Voltage-Regulators/_/N-5cgac?Keyword=TPS76850+SOIC-8&amp;FS=True</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/Optoelectronics/LED-Lighting/LED-Emitters/Standard-LEDs-SMD/_/N-b1bb1</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/Electromechanical/Switches/Pushbutton-Switches/_/N-5g30?P=1z0z7pt&amp;Keyword=button+smd&amp;FS=True</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/All-Manufacturers/_/N-0?Keyword=ULN2003APWR&amp;FS=True</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/_/?Keyword=SFH4545&amp;FS=True</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/ProductDetail/Vishay-Semiconductors/TEFT4300/?qs=HsFHTXumnCRbcrt8oPFPMA%3D%3D</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/ProductDetail/PUI-Audio/SMT-0540-S-R/?qs=%2fha2pyFaduhQZbPx0kWipYmGPvhuTxfaFut09uPs5asFbkbJabBxgw%3d%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/ProductDetail/Micro-Commercial-Components-MCC/1N4148WX-TP/?qs=%2fha2pyFadujM2SPERzkQakcgZq14xl%2f8Qljq0llrhS0%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/Passive-Components/Capacitors/Aluminum-Electrolytic-Capacitors/_/N-75hqt?P=1z0z7ym&amp;Ns=Pricing|0</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/Passive-Components/Inductors-Chokes-Coils/Fixed-Inductors/_/N-wpcz?P=1z0z7ym&amp;Ns=Pricing|0</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/Passive-Components/Resistors/SMD-Resistors-Chip-Resistors/_/N-7h7yu/?Ns=Pricing|0</t>
   </si>
 </sst>
 </file>
@@ -623,7 +653,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Usuario de Microsoft Office" refreshedDate="42820.677499884259" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="37">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Usuario de Microsoft Office" refreshedDate="42883.572925810186" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="37">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabla2"/>
   </cacheSource>
@@ -638,7 +668,7 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Nº" numFmtId="0">
-      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="8"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="10"/>
     </cacheField>
     <cacheField name="Componente" numFmtId="0">
       <sharedItems count="22">
@@ -670,7 +700,7 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Precio" numFmtId="44">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="4.75" maxValue="9.9499999999999993"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.17" maxValue="9.9499999999999993"/>
     </cacheField>
     <cacheField name="Tienda" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -719,8 +749,8 @@
     <n v="6"/>
     <x v="3"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="0.66"/>
+    <s v="http://www.mouser.es/ProductDetail/Vishay-Semiconductors/TEFT4300/?qs=HsFHTXumnCRbcrt8oPFPMA%3D%3D"/>
   </r>
   <r>
     <x v="1"/>
@@ -746,8 +776,8 @@
     <n v="6"/>
     <x v="5"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="0.55000000000000004"/>
+    <s v="http://www.mouser.es/_/?Keyword=SFH4545&amp;FS=True"/>
   </r>
   <r>
     <x v="0"/>
@@ -761,11 +791,11 @@
   <r>
     <x v="0"/>
     <s v="IR EMMITER B)"/>
-    <n v="4"/>
+    <n v="1"/>
     <x v="6"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="0.37"/>
+    <s v="http://www.mouser.es/All-Manufacturers/_/N-0?Keyword=ULN2003APWR&amp;FS=True"/>
   </r>
   <r>
     <x v="0"/>
@@ -773,8 +803,8 @@
     <n v="6"/>
     <x v="5"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="0.55000000000000004"/>
+    <s v="http://www.mouser.es/_/?Keyword=SFH4545&amp;FS=True"/>
   </r>
   <r>
     <x v="0"/>
@@ -791,8 +821,8 @@
     <n v="1"/>
     <x v="8"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="3.3"/>
+    <s v="http://www.mouser.es/ProductDetail/PUI-Audio/SMT-0540-S-R/?qs=%2fha2pyFaduhQZbPx0kWipYmGPvhuTxfaFut09uPs5asFbkbJabBxgw%3d%3d"/>
   </r>
   <r>
     <x v="1"/>
@@ -827,8 +857,8 @@
     <n v="1"/>
     <x v="8"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="3.3"/>
+    <s v="http://www.mouser.es/ProductDetail/PUI-Audio/SMT-0540-S-R/?qs=%2fha2pyFaduhQZbPx0kWipYmGPvhuTxfaFut09uPs5asFbkbJabBxgw%3d%3d"/>
   </r>
   <r>
     <x v="0"/>
@@ -836,8 +866,8 @@
     <n v="1"/>
     <x v="9"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="0.17"/>
+    <s v="http://www.mouser.es/ProductDetail/Micro-Commercial-Components-MCC/1N4148WX-TP/?qs=%2fha2pyFadujM2SPERzkQakcgZq14xl%2f8Qljq0llrhS0%3d"/>
   </r>
   <r>
     <x v="1"/>
@@ -872,8 +902,8 @@
     <n v="1"/>
     <x v="12"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="2.62"/>
+    <s v="http://www.mouser.es/Semiconductors/Power-Management-ICs/Voltage-Regulators-Voltage-Controllers/LDO-Voltage-Regulators/_/N-5cgac?Keyword=TPS76850+SOIC-8&amp;FS=True"/>
   </r>
   <r>
     <x v="0"/>
@@ -881,8 +911,8 @@
     <n v="1"/>
     <x v="13"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="1.88"/>
+    <s v="http://www.mouser.es/_/?Keyword=TPS73633+SOT-23&amp;FS=True"/>
   </r>
   <r>
     <x v="0"/>
@@ -944,13 +974,13 @@
     <n v="1"/>
     <x v="18"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="0.5"/>
+    <s v="http://www.mouser.es/Optoelectronics/LED-Lighting/LED-Emitters/Standard-LEDs-SMD/_/N-b1bb1"/>
   </r>
   <r>
     <x v="0"/>
     <s v="MODE INDICATOR"/>
-    <s v="N"/>
+    <n v="10"/>
     <x v="2"/>
     <m/>
     <m/>
@@ -959,25 +989,25 @@
   <r>
     <x v="0"/>
     <s v="MODE INDICATOR"/>
-    <s v="N"/>
+    <n v="10"/>
     <x v="18"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="0.5"/>
+    <s v="http://www.mouser.es/Optoelectronics/LED-Lighting/LED-Emitters/Standard-LEDs-SMD/_/N-b1bb1"/>
   </r>
   <r>
     <x v="0"/>
     <s v="MODE INDICATOR"/>
-    <s v="M"/>
+    <n v="5"/>
     <x v="19"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="0.5"/>
+    <s v="http://www.mouser.es/Electromechanical/Switches/Pushbutton-Switches/_/N-5g30?P=1z0z7pt&amp;Keyword=button+smd&amp;FS=True"/>
   </r>
   <r>
     <x v="0"/>
     <s v="MODE INDICATOR"/>
-    <s v="M"/>
+    <n v="5"/>
     <x v="2"/>
     <m/>
     <m/>
@@ -1023,7 +1053,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K4:M23" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField name="Selección Componentes:" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -1161,14 +1191,14 @@
     <filterColumn colId="1">
       <filters>
         <filter val="BATERY"/>
-        <filter val="BUZZER A)"/>
+        <filter val="BUZZER B)"/>
         <filter val="GYRO ANALÓGICO"/>
-        <filter val="IR EMMITER A)"/>
+        <filter val="IR EMMITER B)"/>
         <filter val="IR RECEIVER"/>
         <filter val="MICROCONTROLER"/>
         <filter val="MODE INDICATOR"/>
         <filter val="MOTOR DRIVER POLOLU"/>
-        <filter val="POWER SYSTEM A)"/>
+        <filter val="POWER SYSTEM B)"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1449,10 +1479,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="B2:M40"/>
+  <dimension ref="B2:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1462,8 +1492,8 @@
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="4"/>
-    <col min="8" max="8" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="70" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="12.5" customWidth="1"/>
@@ -1471,26 +1501,26 @@
   <sheetData>
     <row r="2" spans="2:13" ht="19" x14ac:dyDescent="0.25">
       <c r="C2" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
       <c r="G2" s="3">
         <f>SUMPRODUCT(Hoja1!$G$4:$G$40, Hoja1!$D$4:$D$40)</f>
-        <v>20.169999999999998</v>
+        <v>57.819999999999986</v>
       </c>
       <c r="H2" s="2"/>
       <c r="K2" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>7</v>
@@ -1512,12 +1542,12 @@
       </c>
       <c r="M3" s="4">
         <f>SUMPRODUCT(M5:M51,L5:L51)</f>
-        <v>20.169999999999998</v>
+        <v>43.769999999999996</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>9</v>
@@ -1536,18 +1566,18 @@
         <v>6</v>
       </c>
       <c r="K4" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" t="s">
         <v>49</v>
-      </c>
-      <c r="L4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>8</v>
@@ -1577,7 +1607,7 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>12</v>
@@ -1589,19 +1619,25 @@
         <v>13</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="K6" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L6" s="5">
-        <v>0</v>
-      </c>
-      <c r="M6" s="19"/>
+        <v>5</v>
+      </c>
+      <c r="M6" s="19">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>12</v>
@@ -1613,19 +1649,25 @@
         <v>14</v>
       </c>
       <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="13"/>
+      <c r="G7" s="14">
+        <v>0.66</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>57</v>
+      </c>
       <c r="K7" s="18" t="s">
         <v>23</v>
       </c>
       <c r="L7" s="5">
         <v>1</v>
       </c>
-      <c r="M7" s="19"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M7" s="19">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>15</v>
@@ -1647,9 +1689,9 @@
       </c>
       <c r="M8" s="19"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>15</v>
@@ -1671,9 +1713,9 @@
       </c>
       <c r="M9" s="19"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>15</v>
@@ -1685,19 +1727,25 @@
         <v>17</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="1"/>
+      <c r="G10" s="16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="K10" s="18" t="s">
         <v>22</v>
       </c>
       <c r="L10" s="5">
         <v>1</v>
       </c>
-      <c r="M10" s="19"/>
-    </row>
-    <row r="11" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M10" s="19">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>18</v>
@@ -1709,8 +1757,12 @@
         <v>13</v>
       </c>
       <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="13"/>
+      <c r="G11" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="K11" s="18" t="s">
         <v>10</v>
       </c>
@@ -1721,24 +1773,28 @@
         <v>5.47</v>
       </c>
     </row>
-    <row r="12" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="1"/>
+      <c r="G12" s="16">
+        <v>0.37</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="K12" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L12" s="5">
         <v>1</v>
@@ -1747,9 +1803,9 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="13" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>18</v>
@@ -1761,8 +1817,12 @@
         <v>17</v>
       </c>
       <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="13"/>
+      <c r="G13" s="16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="K13" s="18" t="s">
         <v>31</v>
       </c>
@@ -1771,9 +1831,9 @@
       </c>
       <c r="M13" s="19"/>
     </row>
-    <row r="14" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>18</v>
@@ -1785,19 +1845,25 @@
         <v>20</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="1"/>
+      <c r="G14" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="K14" s="18" t="s">
         <v>17</v>
       </c>
       <c r="L14" s="5">
         <v>6</v>
       </c>
-      <c r="M14" s="19"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M14" s="19">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>21</v>
@@ -1809,19 +1875,25 @@
         <v>23</v>
       </c>
       <c r="F15" s="13"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="13"/>
+      <c r="G15" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>58</v>
+      </c>
       <c r="K15" s="18" t="s">
         <v>14</v>
       </c>
       <c r="L15" s="5">
         <v>6</v>
       </c>
-      <c r="M15" s="19"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M15" s="19">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>21</v>
@@ -1836,16 +1908,18 @@
       <c r="G16" s="16"/>
       <c r="H16" s="1"/>
       <c r="K16" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L16" s="5">
-        <v>1</v>
-      </c>
-      <c r="M16" s="19"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="M16" s="19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>21</v>
@@ -1860,16 +1934,16 @@
       <c r="G17" s="14"/>
       <c r="H17" s="13"/>
       <c r="K17" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L17" s="5">
         <v>1</v>
       </c>
       <c r="M17" s="19"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>21</v>
@@ -1887,13 +1961,13 @@
         <v>13</v>
       </c>
       <c r="L18" s="5">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="M18" s="19"/>
     </row>
-    <row r="19" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>24</v>
@@ -1905,8 +1979,12 @@
         <v>23</v>
       </c>
       <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="13"/>
+      <c r="G19" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>58</v>
+      </c>
       <c r="K19" s="18" t="s">
         <v>32</v>
       </c>
@@ -1915,9 +1993,9 @@
       </c>
       <c r="M19" s="19"/>
     </row>
-    <row r="20" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>24</v>
@@ -1929,8 +2007,12 @@
         <v>22</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="1"/>
+      <c r="G20" s="16">
+        <v>0.17</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="K20" s="18" t="s">
         <v>35</v>
       </c>
@@ -1939,9 +2021,9 @@
       </c>
       <c r="M20" s="19"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>25</v>
@@ -1961,11 +2043,13 @@
       <c r="L21" s="5">
         <v>1</v>
       </c>
-      <c r="M21" s="19"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M21" s="19">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>25</v>
@@ -1985,11 +2069,13 @@
       <c r="L22" s="5">
         <v>1</v>
       </c>
-      <c r="M22" s="19"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M22" s="19">
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>25</v>
@@ -2007,13 +2093,15 @@
         <v>19</v>
       </c>
       <c r="L23" s="5">
-        <v>4</v>
-      </c>
-      <c r="M23" s="19"/>
-    </row>
-    <row r="24" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="M23" s="19">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>28</v>
@@ -2025,12 +2113,16 @@
         <v>29</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G24" s="16">
+        <v>2.62</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>28</v>
@@ -2042,12 +2134,16 @@
         <v>30</v>
       </c>
       <c r="F25" s="13"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="13"/>
-    </row>
-    <row r="26" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G25" s="14">
+        <v>1.88</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>28</v>
@@ -2059,12 +2155,16 @@
         <v>20</v>
       </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G26" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>28</v>
@@ -2076,12 +2176,16 @@
         <v>31</v>
       </c>
       <c r="F27" s="13"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="13"/>
-    </row>
-    <row r="28" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G27" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>28</v>
@@ -2093,12 +2197,16 @@
         <v>32</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="1"/>
+      <c r="G28" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>33</v>
@@ -2115,7 +2223,7 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>33</v>
@@ -2127,12 +2235,16 @@
         <v>35</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="1"/>
+      <c r="G30" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>33</v>
@@ -2144,12 +2256,16 @@
         <v>13</v>
       </c>
       <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="13"/>
+      <c r="G31" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>33</v>
@@ -2158,107 +2274,127 @@
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F32" s="1"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="1"/>
+      <c r="G32" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="13" t="s">
-        <v>37</v>
+      <c r="D33" s="13">
+        <v>10</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="13"/>
+      <c r="G33" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>37</v>
+      <c r="D34" s="1">
+        <v>10</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F34" s="1"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="1"/>
+      <c r="G34" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="13" t="s">
-        <v>38</v>
+      <c r="D35" s="13">
+        <v>5</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F35" s="13"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="13"/>
+      <c r="G35" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>38</v>
+      <c r="D36" s="1">
+        <v>5</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="1"/>
+      <c r="G36" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D37" s="13">
         <v>1</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F37" s="13"/>
       <c r="G37" s="14">
         <v>4.75</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D38" s="1">
         <v>3</v>
@@ -2267,32 +2403,40 @@
         <v>13</v>
       </c>
       <c r="F38" s="1"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="1"/>
+      <c r="G38" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D39" s="13">
         <v>1</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F39" s="13"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="13"/>
+      <c r="G39" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D40" s="1">
         <v>2</v>
@@ -2301,8 +2445,18 @@
         <v>20</v>
       </c>
       <c r="F40" s="1"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="1"/>
+      <c r="G40" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G41" s="4">
+        <f>SUMPRODUCT(G6:G36,D6:D36)</f>
+        <v>36.550000000000004</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
esquematico finalizado. Componentes colocados. Comienzo del enrutado.
</commit_message>
<xml_diff>
--- a/Componentes.xlsx
+++ b/Componentes.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" calcMode="manual" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="67">
   <si>
     <t>Componente</t>
   </si>
@@ -216,6 +216,18 @@
   </si>
   <si>
     <t>http://www.mouser.es/Passive-Components/Resistors/SMD-Resistors-Chip-Resistors/_/N-7h7yu/?Ns=Pricing|0</t>
+  </si>
+  <si>
+    <t>http://www.mouser.es/ProductDetail/Infineon/IRLML6344TRPBF/?qs=%2fha2pyFadug9a5KeKuUVDnkcuanTRcw4TBT4CWZt5Hy0rA%252b6q2Axjw%3d%3d</t>
+  </si>
+  <si>
+    <t>1,8k</t>
+  </si>
+  <si>
+    <t>10ohm</t>
+  </si>
+  <si>
+    <t>1k</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1065,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K4:M23" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField name="Selección Componentes:" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -1191,13 +1203,14 @@
     <filterColumn colId="1">
       <filters>
         <filter val="BATERY"/>
-        <filter val="BUZZER B)"/>
+        <filter val="BUZZER A)"/>
         <filter val="GYRO ANALÓGICO"/>
-        <filter val="IR EMMITER B)"/>
+        <filter val="IR EMMITER A)"/>
         <filter val="IR RECEIVER"/>
         <filter val="MICROCONTROLER"/>
         <filter val="MODE INDICATOR"/>
         <filter val="MOTOR DRIVER POLOLU"/>
+        <filter val="POWER SYSTEM A)"/>
         <filter val="POWER SYSTEM B)"/>
       </filters>
     </filterColumn>
@@ -1479,10 +1492,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="B2:M41"/>
+  <dimension ref="B2:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1508,7 +1521,7 @@
       <c r="F2" s="20"/>
       <c r="G2" s="3">
         <f>SUMPRODUCT(Hoja1!$G$4:$G$40, Hoja1!$D$4:$D$40)</f>
-        <v>57.819999999999986</v>
+        <v>58.389999999999986</v>
       </c>
       <c r="H2" s="2"/>
       <c r="K2" s="17" t="s">
@@ -1665,7 +1678,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="8" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>46</v>
       </c>
@@ -1689,7 +1702,7 @@
       </c>
       <c r="M8" s="19"/>
     </row>
-    <row r="9" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>46</v>
       </c>
@@ -1713,7 +1726,7 @@
       </c>
       <c r="M9" s="19"/>
     </row>
-    <row r="10" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>46</v>
       </c>
@@ -1743,7 +1756,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>45</v>
       </c>
@@ -1773,7 +1786,7 @@
         <v>5.47</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>45</v>
       </c>
@@ -1803,7 +1816,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>45</v>
       </c>
@@ -1831,7 +1844,7 @@
       </c>
       <c r="M13" s="19"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>45</v>
       </c>
@@ -1861,7 +1874,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="15" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>46</v>
       </c>
@@ -1891,7 +1904,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="16" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>46</v>
       </c>
@@ -1905,8 +1918,12 @@
         <v>22</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="1"/>
+      <c r="G16" s="16">
+        <v>0.17</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="K16" s="18" t="s">
         <v>38</v>
       </c>
@@ -1917,7 +1934,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>46</v>
       </c>
@@ -1931,8 +1948,12 @@
         <v>16</v>
       </c>
       <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="13"/>
+      <c r="G17" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>63</v>
+      </c>
       <c r="K17" s="18" t="s">
         <v>42</v>
       </c>
@@ -1941,7 +1962,7 @@
       </c>
       <c r="M17" s="19"/>
     </row>
-    <row r="18" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>46</v>
       </c>
@@ -1965,7 +1986,7 @@
       </c>
       <c r="M18" s="19"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>45</v>
       </c>
@@ -1993,7 +2014,7 @@
       </c>
       <c r="M19" s="19"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>45</v>
       </c>
@@ -2021,7 +2042,7 @@
       </c>
       <c r="M20" s="19"/>
     </row>
-    <row r="21" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>46</v>
       </c>
@@ -2047,7 +2068,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="22" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>46</v>
       </c>
@@ -2073,7 +2094,7 @@
         <v>2.62</v>
       </c>
     </row>
-    <row r="23" spans="2:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>46</v>
       </c>
@@ -2455,7 +2476,25 @@
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G41" s="4">
         <f>SUMPRODUCT(G6:G36,D6:D36)</f>
-        <v>36.550000000000004</v>
+        <v>37.120000000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>805</v>
+      </c>
+      <c r="F43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F44" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>